<commit_message>
4/9/2020  capture direcory name change.  project file. review doc
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/JavaScriptFrameDistillationToTheFinish_v3.xlsx
+++ b/CurrentWork_Delta/JavaScriptFrameDistillationToTheFinish_v3.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mark\CurrentWork_Delta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A5BBF1-2C82-4B7A-8473-BC48727B5F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3734F25E-0F3C-4823-A633-38AECCB99E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20160" yWindow="945" windowWidth="16845" windowHeight="15435" xr2:uid="{1C02CC31-4B62-49F7-B75D-EAE54FAFEDF3}"/>
+    <workbookView xWindow="8595" yWindow="930" windowWidth="20925" windowHeight="16830" activeTab="2" xr2:uid="{1C02CC31-4B62-49F7-B75D-EAE54FAFEDF3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Current" sheetId="1" r:id="rId1"/>
-    <sheet name="Previous" sheetId="2" r:id="rId2"/>
+    <sheet name="initial PLan" sheetId="2" r:id="rId1"/>
+    <sheet name="Adopted Plan" sheetId="1" r:id="rId2"/>
+    <sheet name="Current State" sheetId="4" r:id="rId3"/>
+    <sheet name="Accomplishment" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
   <si>
     <t>Expand Unit Test Runs to generate rpt data</t>
   </si>
@@ -282,13 +284,90 @@
   </si>
   <si>
     <t xml:space="preserve">   Document strucural change seperating Frame from App specific code.</t>
+  </si>
+  <si>
+    <t>Tuesday March 24 2020</t>
+  </si>
+  <si>
+    <t>Following a constructive call with CU</t>
+  </si>
+  <si>
+    <t>Reviewed the nature of the two functions in Ramdom.js  randomNo and randomTestVal()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RandomNo was found un used throughout the entire product test environment.  I deprecated randonNo by commenting out.  </t>
+  </si>
+  <si>
+    <t>RandomTestVal  is in the proces of being refactored and new functions are being reconnected to previous calling locations.   New fuctions are atomic and somewhat less error prone to call.</t>
+  </si>
+  <si>
+    <t>New functions are 
+     randomTestSTRING(n); requires length of string to return
+     randomTestDATE();        no argument</t>
+  </si>
+  <si>
+    <t>randomeTestSTRING function has at least one unit test / functional test implemented via a call from pageTest\getAQuote\delta\basicPlus.test.js line 93 in function  it('Unit Test: Access Random.js.randomTestSTRING ', function()     
+Additionally pageObject\dependent-page.js  also maks calls to randomeTestSTRING at lines 351&amp;352</t>
+  </si>
+  <si>
+    <t>Lastly, all current Framework Unit tests run and pass without error</t>
+  </si>
+  <si>
+    <t>Identified work completed</t>
+  </si>
+  <si>
+    <t>Identified work that needs attention</t>
+  </si>
+  <si>
+    <t>It looks like I should implement something like pageTests\dependents\delta\basic.test.js ..  The deal is that there is a great deal of work just to have a position for adding dependents with CHILDDOB , the newest Random.js  function.  Will consider other alternatives like a page that already exist that needs just a little help getting there.</t>
+  </si>
+  <si>
+    <t>The following two files and managed functions 
+Dates
+     GetDatePart only called by a function that is not used at all
+     getFullDate  was not called by anything
+Files
+     readPDFFiles  is no longer used in any JS framework
+     renameReports   while there are two calls in the ESS Test
+     framework.  Since I am not forcing any frame to adopt the new core
+     ESS Can for the time being continue useing renameReports as it it.</t>
+  </si>
+  <si>
+    <t>Recommended changes across the JS Frame user base</t>
+  </si>
+  <si>
+    <t>At some point in the near future the ESS framwork need to have the 
+Cole/MarketPlace/Core Test Reporting frame work adopted.</t>
+  </si>
+  <si>
+    <t>3/27/2020
+Moving logInfoPromise to ViewPort.js from Errors.  
+Errors.js was an arbitrary place when deprecating common.js  So, ViewPort.js is just as reasonable from that stand point.  But more to how the function is used via lexical Scope use of 'this' and not thorough a Global Variable like Uitlity was used for, logInfoPromise belong in the same file that calles it.</t>
+  </si>
+  <si>
+    <t>3/30/2020
+it turns out that using the end to end framework to access all pages just requires too much of the Applicaiotn specific code into what I want to be just frame work.  So, my ability to unit test Core functions by navigating over application pages will not keep the core clean.  So, I will have to use the Jasmine methodology to unit test core code.</t>
+  </si>
+  <si>
+    <t>3/30/2020
+I believe there is a snag in the reporting framework.
+When I run ./go 3 and run three suites in parallel I get one output folder , I get three json file, but only one report.  The json files are named by the process id running.  I'm looking at the methodology for reporting to determine if I can get it to gen the html for all json generated.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>50% done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +394,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,13 +460,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,409 +781,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCB175D-C41E-43F0-A193-CDB42C3700EA}">
-  <dimension ref="A1:H44"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" style="2" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="2.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D1" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="9">
-        <v>43907</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7">
-        <v>3</v>
-      </c>
-      <c r="F5" s="10">
-        <f>WORKDAY.INTL(D2,E5)</f>
-        <v>43910</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="7">
-        <v>2</v>
-      </c>
-      <c r="F10" s="10">
-        <f>WORKDAY.INTL(F5,E10)</f>
-        <v>43914</v>
-      </c>
-      <c r="H10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="14"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="7">
-        <v>5</v>
-      </c>
-      <c r="F15" s="10">
-        <f>WORKDAY.INTL(F10,E15)</f>
-        <v>43921</v>
-      </c>
-      <c r="H15" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="7">
-        <v>4</v>
-      </c>
-      <c r="F21" s="10">
-        <f>WORKDAY.INTL(F15,E21)</f>
-        <v>43927</v>
-      </c>
-      <c r="H21" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="9">
-        <v>43928</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E32" s="7"/>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="7">
-        <v>6</v>
-      </c>
-      <c r="F33" s="10">
-        <f>IF(ISBLANK($D$31),"",WORKDAY.INTL(D31,E33))</f>
-        <v>43936</v>
-      </c>
-      <c r="H33" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="10"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="10"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E38" s="7"/>
-      <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E39" s="7"/>
-      <c r="F39" s="10"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="7">
-        <v>3</v>
-      </c>
-      <c r="F40" s="10">
-        <f>IF(ISBLANK($D$31),"",WORKDAY.INTL(F33,E40))</f>
-        <v>43941</v>
-      </c>
-      <c r="H40" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F42" s="10"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E43" s="7"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E44" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCAF22A-84AA-4DB0-AA46-3F2E574E7ABB}">
   <dimension ref="B2:H47"/>
   <sheetViews>
@@ -1380,4 +1062,962 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCB175D-C41E-43F0-A193-CDB42C3700EA}">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="9">
+        <v>43907</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10">
+        <f>WORKDAY.INTL(D2,E5)</f>
+        <v>43910</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="10">
+        <f>WORKDAY.INTL(F5,E10)</f>
+        <v>43914</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="7">
+        <v>5</v>
+      </c>
+      <c r="F15" s="10">
+        <f>WORKDAY.INTL(F10,E15)</f>
+        <v>43921</v>
+      </c>
+      <c r="H15" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4</v>
+      </c>
+      <c r="F21" s="10">
+        <f>WORKDAY.INTL(F15,E21)</f>
+        <v>43927</v>
+      </c>
+      <c r="H21" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="9">
+        <v>43928</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E32" s="7"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="7">
+        <v>6</v>
+      </c>
+      <c r="F33" s="10">
+        <f>IF(ISBLANK($D$31),"",WORKDAY.INTL(D31,E33))</f>
+        <v>43936</v>
+      </c>
+      <c r="H33" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E38" s="7"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E39" s="7"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="7">
+        <v>3</v>
+      </c>
+      <c r="F40" s="10">
+        <f>IF(ISBLANK($D$31),"",WORKDAY.INTL(F33,E40))</f>
+        <v>43941</v>
+      </c>
+      <c r="H40" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E43" s="7"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E44" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3754D3-B842-4BBE-8175-10B182BDC6BC}">
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="9">
+        <v>43907</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10">
+        <f>WORKDAY.INTL(D2,E5)</f>
+        <v>43910</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10">
+        <f>WORKDAY.INTL(F5,E12)</f>
+        <v>43914</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="13"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="7">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10">
+        <f>WORKDAY.INTL(F12,E17)</f>
+        <v>43921</v>
+      </c>
+      <c r="H17" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="7">
+        <v>4</v>
+      </c>
+      <c r="F23" s="10">
+        <f>WORKDAY.INTL(F17,E23)</f>
+        <v>43927</v>
+      </c>
+      <c r="H23" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="9">
+        <v>43928</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E36" s="7"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="7">
+        <v>6</v>
+      </c>
+      <c r="F37" s="10">
+        <f>IF(ISBLANK($D$35),"",WORKDAY.INTL(D35,E37))</f>
+        <v>43936</v>
+      </c>
+      <c r="H37" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E42" s="7"/>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E43" s="7"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="7">
+        <v>3</v>
+      </c>
+      <c r="F44" s="10">
+        <f>IF(ISBLANK($D$35),"",WORKDAY.INTL(F37,E44))</f>
+        <v>43941</v>
+      </c>
+      <c r="H44" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E47" s="7"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E48" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7387394D-B48D-41AE-BB9F-DA01136C2CD2}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="62.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="67.28515625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>43914</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>43917</v>
+      </c>
+      <c r="D13" s="9">
+        <v>43915</v>
+      </c>
+      <c r="E13" s="10">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="159" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>